<commit_message>
resolves #49 :tractor: :sparkles: :hammer: :microscope:
</commit_message>
<xml_diff>
--- a/SonghayCore.Tests/xlsx/latin-glyphs.xlsx
+++ b/SonghayCore.Tests/xlsx/latin-glyphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~shares\sourceRoot\SonghayCore\SonghayCore.Tests\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94F160D-85F3-4B69-BA31-AD12D0F55E04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1520FA8E-27D7-41FB-B175-885228AA55C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28980" yWindow="465" windowWidth="28530" windowHeight="14910" xr2:uid="{37D4E14C-789D-4D3D-87AC-A7379466EBE7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="850">
   <si>
     <t>Character</t>
   </si>
@@ -2580,9 +2580,6 @@
   </si>
   <si>
     <t>20</t>
-  </si>
-  <si>
-    <t>C# Tuple Pair</t>
   </si>
   <si>
     <t>22</t>
@@ -3047,11 +3044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624E43A4-11C6-4DF9-8BF5-916BD7383648}">
-  <dimension ref="A1:I225"/>
+  <dimension ref="A1:H225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -3063,12 +3059,11 @@
     <col min="5" max="5" width="24" style="3" customWidth="1"/>
     <col min="6" max="6" width="35.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="34.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="249.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="61.140625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="8" max="8" width="61.140625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>625</v>
       </c>
@@ -3090,14 +3085,11 @@
       <c r="G1" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>849</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>848</v>
       </c>
@@ -3118,15 +3110,11 @@
         <f>_xlfn.CONCAT("&amp;#",HEX2DEC(A2),";")</f>
         <v>&amp;#32;</v>
       </c>
-      <c r="H2" s="7" t="str">
-        <f>_xlfn.CONCAT("{ """, A2, """, ( Character: """, _xlfn.SWITCH(A2, "22", "\""", "5c", "\\", C2), """, Windows1252UrlEncoding: """, D2, """, Utf8Encoding: """, E2, """, HtmlEntityName: """, F2, """, XmlEntityNumber: """, G2, """ ) },")</f>
-        <v>{ "20", ( Character: " ", Windows1252UrlEncoding: "%20", Utf8Encoding: "%20", HtmlEntityName: "", XmlEntityNumber: "&amp;#32;" ) },</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>21</v>
       </c>
@@ -3147,17 +3135,13 @@
         <f t="shared" ref="G3:G66" si="0">_xlfn.CONCAT("&amp;#",HEX2DEC(A3),";")</f>
         <v>&amp;#33;</v>
       </c>
-      <c r="H3" s="8" t="str">
-        <f t="shared" ref="H3:H66" si="1">_xlfn.CONCAT("{ """, A3, """, ( Character: """, _xlfn.SWITCH(A3, "22", "\""", "5c", "\\", C3), """, Windows1252UrlEncoding: """, D3, """, Utf8Encoding: """, E3, """, HtmlEntityName: """, F3, """, XmlEntityNumber: """, G3, """ ) },")</f>
-        <v>{ "21", ( Character: "!", Windows1252UrlEncoding: "%21", Utf8Encoding: "%21", HtmlEntityName: "", XmlEntityNumber: "&amp;#33;" ) },</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>830</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>840</v>
@@ -3178,15 +3162,11 @@
         <f t="shared" si="0"/>
         <v>&amp;#34;</v>
       </c>
-      <c r="H4" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "22", ( Character: "\"", Windows1252UrlEncoding: "%22", Utf8Encoding: "%22", HtmlEntityName: "&amp;quot;", XmlEntityNumber: "&amp;#34;" ) },</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>23</v>
       </c>
@@ -3207,12 +3187,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#35;</v>
       </c>
-      <c r="H5" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "23", ( Character: "#", Windows1252UrlEncoding: "%23", Utf8Encoding: "%23", HtmlEntityName: "", XmlEntityNumber: "&amp;#35;" ) },</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>24</v>
       </c>
@@ -3233,12 +3209,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#36;</v>
       </c>
-      <c r="H6" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "24", ( Character: "$", Windows1252UrlEncoding: "%24", Utf8Encoding: "%24", HtmlEntityName: "", XmlEntityNumber: "&amp;#36;" ) },</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>25</v>
       </c>
@@ -3259,12 +3231,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#37;</v>
       </c>
-      <c r="H7" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "25", ( Character: "%", Windows1252UrlEncoding: "%25", Utf8Encoding: "%25", HtmlEntityName: "", XmlEntityNumber: "&amp;#37;" ) },</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>26</v>
       </c>
@@ -3287,12 +3255,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#38;</v>
       </c>
-      <c r="H8" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "26", ( Character: "&amp;", Windows1252UrlEncoding: "%26", Utf8Encoding: "%26", HtmlEntityName: "&amp;amp;", XmlEntityNumber: "&amp;#38;" ) },</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>27</v>
       </c>
@@ -3315,12 +3279,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#39;</v>
       </c>
-      <c r="H9" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "27", ( Character: "'", Windows1252UrlEncoding: "%27", Utf8Encoding: "%27", HtmlEntityName: "	&amp;apos;", XmlEntityNumber: "&amp;#39;" ) },</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>28</v>
       </c>
@@ -3341,12 +3301,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#40;</v>
       </c>
-      <c r="H10" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "28", ( Character: "(", Windows1252UrlEncoding: "%28", Utf8Encoding: "%28", HtmlEntityName: "", XmlEntityNumber: "&amp;#40;" ) },</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>29</v>
       </c>
@@ -3367,12 +3323,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#41;</v>
       </c>
-      <c r="H11" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "29", ( Character: ")", Windows1252UrlEncoding: "%29", Utf8Encoding: "%29", HtmlEntityName: "", XmlEntityNumber: "&amp;#41;" ) },</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>484</v>
       </c>
@@ -3393,12 +3345,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#42;</v>
       </c>
-      <c r="H12" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "2a", ( Character: "*", Windows1252UrlEncoding: "%2A", Utf8Encoding: "%2A", HtmlEntityName: "", XmlEntityNumber: "&amp;#42;" ) },</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>485</v>
       </c>
@@ -3419,12 +3367,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#43;</v>
       </c>
-      <c r="H13" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "2b", ( Character: "+", Windows1252UrlEncoding: "%2B", Utf8Encoding: "%2B", HtmlEntityName: "", XmlEntityNumber: "&amp;#43;" ) },</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>486</v>
       </c>
@@ -3445,12 +3389,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#44;</v>
       </c>
-      <c r="H14" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "2c", ( Character: ",", Windows1252UrlEncoding: "%2C", Utf8Encoding: "%2C", HtmlEntityName: "", XmlEntityNumber: "&amp;#44;" ) },</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>487</v>
       </c>
@@ -3471,12 +3411,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#45;</v>
       </c>
-      <c r="H15" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "2d", ( Character: "-", Windows1252UrlEncoding: "%2D", Utf8Encoding: "%2D", HtmlEntityName: "", XmlEntityNumber: "&amp;#45;" ) },</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>488</v>
       </c>
@@ -3497,12 +3433,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#46;</v>
       </c>
-      <c r="H16" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "2e", ( Character: ".", Windows1252UrlEncoding: "%2E", Utf8Encoding: "%2E", HtmlEntityName: "", XmlEntityNumber: "&amp;#46;" ) },</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>489</v>
       </c>
@@ -3523,12 +3455,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#47;</v>
       </c>
-      <c r="H17" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "2f", ( Character: "/", Windows1252UrlEncoding: "%2F", Utf8Encoding: "%2F", HtmlEntityName: "", XmlEntityNumber: "&amp;#47;" ) },</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>30</v>
       </c>
@@ -3549,12 +3477,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#48;</v>
       </c>
-      <c r="H18" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "30", ( Character: "0", Windows1252UrlEncoding: "%30", Utf8Encoding: "%30", HtmlEntityName: "", XmlEntityNumber: "&amp;#48;" ) },</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>31</v>
       </c>
@@ -3575,12 +3499,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#49;</v>
       </c>
-      <c r="H19" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "31", ( Character: "1", Windows1252UrlEncoding: "%31", Utf8Encoding: "%31", HtmlEntityName: "", XmlEntityNumber: "&amp;#49;" ) },</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>32</v>
       </c>
@@ -3601,12 +3521,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#50;</v>
       </c>
-      <c r="H20" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "32", ( Character: "2", Windows1252UrlEncoding: "%32", Utf8Encoding: "%32", HtmlEntityName: "", XmlEntityNumber: "&amp;#50;" ) },</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>33</v>
       </c>
@@ -3627,12 +3543,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#51;</v>
       </c>
-      <c r="H21" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "33", ( Character: "3", Windows1252UrlEncoding: "%33", Utf8Encoding: "%33", HtmlEntityName: "", XmlEntityNumber: "&amp;#51;" ) },</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>34</v>
       </c>
@@ -3653,12 +3565,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#52;</v>
       </c>
-      <c r="H22" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "34", ( Character: "4", Windows1252UrlEncoding: "%34", Utf8Encoding: "%34", HtmlEntityName: "", XmlEntityNumber: "&amp;#52;" ) },</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>35</v>
       </c>
@@ -3679,12 +3587,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#53;</v>
       </c>
-      <c r="H23" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "35", ( Character: "5", Windows1252UrlEncoding: "%35", Utf8Encoding: "%35", HtmlEntityName: "", XmlEntityNumber: "&amp;#53;" ) },</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>36</v>
       </c>
@@ -3705,12 +3609,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#54;</v>
       </c>
-      <c r="H24" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "36", ( Character: "6", Windows1252UrlEncoding: "%36", Utf8Encoding: "%36", HtmlEntityName: "", XmlEntityNumber: "&amp;#54;" ) },</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
         <v>37</v>
       </c>
@@ -3731,12 +3631,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#55;</v>
       </c>
-      <c r="H25" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "37", ( Character: "7", Windows1252UrlEncoding: "%37", Utf8Encoding: "%37", HtmlEntityName: "", XmlEntityNumber: "&amp;#55;" ) },</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>38</v>
       </c>
@@ -3757,12 +3653,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#56;</v>
       </c>
-      <c r="H26" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "38", ( Character: "8", Windows1252UrlEncoding: "%38", Utf8Encoding: "%38", HtmlEntityName: "", XmlEntityNumber: "&amp;#56;" ) },</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="5">
         <v>39</v>
       </c>
@@ -3783,12 +3675,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#57;</v>
       </c>
-      <c r="H27" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "39", ( Character: "9", Windows1252UrlEncoding: "%39", Utf8Encoding: "%39", HtmlEntityName: "", XmlEntityNumber: "&amp;#57;" ) },</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>490</v>
       </c>
@@ -3809,12 +3697,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#58;</v>
       </c>
-      <c r="H28" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "3a", ( Character: ":", Windows1252UrlEncoding: "%3A", Utf8Encoding: "%3A", HtmlEntityName: "", XmlEntityNumber: "&amp;#58;" ) },</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>491</v>
       </c>
@@ -3835,12 +3719,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#59;</v>
       </c>
-      <c r="H29" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "3b", ( Character: ";", Windows1252UrlEncoding: "%3B", Utf8Encoding: "%3B", HtmlEntityName: "", XmlEntityNumber: "&amp;#59;" ) },</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
         <v>492</v>
       </c>
@@ -3863,12 +3743,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#60;</v>
       </c>
-      <c r="H30" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "3c", ( Character: "&lt;", Windows1252UrlEncoding: "%3C", Utf8Encoding: "%3C", HtmlEntityName: "	&amp;lt;", XmlEntityNumber: "&amp;#60;" ) },</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>493</v>
       </c>
@@ -3889,12 +3765,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#61;</v>
       </c>
-      <c r="H31" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "3d", ( Character: "=", Windows1252UrlEncoding: "%3D", Utf8Encoding: "%3D", HtmlEntityName: "", XmlEntityNumber: "&amp;#61;" ) },</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
         <v>494</v>
       </c>
@@ -3917,12 +3789,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#62;</v>
       </c>
-      <c r="H32" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "3e", ( Character: "&gt;", Windows1252UrlEncoding: "%3E", Utf8Encoding: "%3E", HtmlEntityName: "&amp;gt;", XmlEntityNumber: "&amp;#62;" ) },</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>495</v>
       </c>
@@ -3943,12 +3811,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#63;</v>
       </c>
-      <c r="H33" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "3f", ( Character: "?", Windows1252UrlEncoding: "%3F", Utf8Encoding: "%3F", HtmlEntityName: "", XmlEntityNumber: "&amp;#63;" ) },</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>40</v>
       </c>
@@ -3969,12 +3833,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#64;</v>
       </c>
-      <c r="H34" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "40", ( Character: "@", Windows1252UrlEncoding: "%40", Utf8Encoding: "%40", HtmlEntityName: "", XmlEntityNumber: "&amp;#64;" ) },</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="5">
         <v>41</v>
       </c>
@@ -3995,12 +3855,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#65;</v>
       </c>
-      <c r="H35" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "41", ( Character: "A", Windows1252UrlEncoding: "%41", Utf8Encoding: "%41", HtmlEntityName: "", XmlEntityNumber: "&amp;#65;" ) },</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
         <v>42</v>
       </c>
@@ -4021,12 +3877,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#66;</v>
       </c>
-      <c r="H36" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "42", ( Character: "B", Windows1252UrlEncoding: "%42", Utf8Encoding: "%42", HtmlEntityName: "", XmlEntityNumber: "&amp;#66;" ) },</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" s="5">
         <v>43</v>
       </c>
@@ -4047,12 +3899,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#67;</v>
       </c>
-      <c r="H37" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "43", ( Character: "C", Windows1252UrlEncoding: "%43", Utf8Encoding: "%43", HtmlEntityName: "", XmlEntityNumber: "&amp;#67;" ) },</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>44</v>
       </c>
@@ -4073,12 +3921,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#68;</v>
       </c>
-      <c r="H38" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "44", ( Character: "D", Windows1252UrlEncoding: "%44", Utf8Encoding: "%44", HtmlEntityName: "", XmlEntityNumber: "&amp;#68;" ) },</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="5">
         <v>45</v>
       </c>
@@ -4099,12 +3943,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#69;</v>
       </c>
-      <c r="H39" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "45", ( Character: "E", Windows1252UrlEncoding: "%45", Utf8Encoding: "%45", HtmlEntityName: "", XmlEntityNumber: "&amp;#69;" ) },</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="40" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="4">
         <v>46</v>
       </c>
@@ -4125,12 +3965,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#70;</v>
       </c>
-      <c r="H40" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "46", ( Character: "F", Windows1252UrlEncoding: "%46", Utf8Encoding: "%46", HtmlEntityName: "", XmlEntityNumber: "&amp;#70;" ) },</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="41" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A41" s="5">
         <v>47</v>
       </c>
@@ -4151,12 +3987,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#71;</v>
       </c>
-      <c r="H41" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "47", ( Character: "G", Windows1252UrlEncoding: "%47", Utf8Encoding: "%47", HtmlEntityName: "", XmlEntityNumber: "&amp;#71;" ) },</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="42" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A42" s="4">
         <v>48</v>
       </c>
@@ -4177,12 +4009,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#72;</v>
       </c>
-      <c r="H42" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "48", ( Character: "H", Windows1252UrlEncoding: "%48", Utf8Encoding: "%48", HtmlEntityName: "", XmlEntityNumber: "&amp;#72;" ) },</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A43" s="5">
         <v>49</v>
       </c>
@@ -4203,12 +4031,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#73;</v>
       </c>
-      <c r="H43" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "49", ( Character: "I", Windows1252UrlEncoding: "%49", Utf8Encoding: "%49", HtmlEntityName: "", XmlEntityNumber: "&amp;#73;" ) },</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="44" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
         <v>496</v>
       </c>
@@ -4229,12 +4053,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#74;</v>
       </c>
-      <c r="H44" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "4a", ( Character: "J", Windows1252UrlEncoding: "%4A", Utf8Encoding: "%4A", HtmlEntityName: "", XmlEntityNumber: "&amp;#74;" ) },</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="45" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" s="5" t="s">
         <v>497</v>
       </c>
@@ -4255,12 +4075,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#75;</v>
       </c>
-      <c r="H45" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "4b", ( Character: "K", Windows1252UrlEncoding: "%4B", Utf8Encoding: "%4B", HtmlEntityName: "", XmlEntityNumber: "&amp;#75;" ) },</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="46" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
         <v>498</v>
       </c>
@@ -4281,12 +4097,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#76;</v>
       </c>
-      <c r="H46" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "4c", ( Character: "L", Windows1252UrlEncoding: "%4C", Utf8Encoding: "%4C", HtmlEntityName: "", XmlEntityNumber: "&amp;#76;" ) },</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="47" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A47" s="5" t="s">
         <v>499</v>
       </c>
@@ -4307,12 +4119,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#77;</v>
       </c>
-      <c r="H47" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "4d", ( Character: "M", Windows1252UrlEncoding: "%4D", Utf8Encoding: "%4D", HtmlEntityName: "", XmlEntityNumber: "&amp;#77;" ) },</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="48" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
         <v>500</v>
       </c>
@@ -4333,12 +4141,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#78;</v>
       </c>
-      <c r="H48" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "4e", ( Character: "N", Windows1252UrlEncoding: "%4E", Utf8Encoding: "%4E", HtmlEntityName: "", XmlEntityNumber: "&amp;#78;" ) },</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="49" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A49" s="5" t="s">
         <v>501</v>
       </c>
@@ -4359,12 +4163,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#79;</v>
       </c>
-      <c r="H49" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "4f", ( Character: "O", Windows1252UrlEncoding: "%4F", Utf8Encoding: "%4F", HtmlEntityName: "", XmlEntityNumber: "&amp;#79;" ) },</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="50" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A50" s="4">
         <v>50</v>
       </c>
@@ -4385,12 +4185,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#80;</v>
       </c>
-      <c r="H50" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "50", ( Character: "P", Windows1252UrlEncoding: "%50", Utf8Encoding: "%50", HtmlEntityName: "", XmlEntityNumber: "&amp;#80;" ) },</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="51" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A51" s="5">
         <v>51</v>
       </c>
@@ -4411,12 +4207,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#81;</v>
       </c>
-      <c r="H51" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "51", ( Character: "Q", Windows1252UrlEncoding: "%51", Utf8Encoding: "%51", HtmlEntityName: "", XmlEntityNumber: "&amp;#81;" ) },</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="52" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A52" s="4">
         <v>52</v>
       </c>
@@ -4437,12 +4229,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#82;</v>
       </c>
-      <c r="H52" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "52", ( Character: "R", Windows1252UrlEncoding: "%52", Utf8Encoding: "%52", HtmlEntityName: "", XmlEntityNumber: "&amp;#82;" ) },</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="53" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A53" s="5">
         <v>53</v>
       </c>
@@ -4463,12 +4251,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#83;</v>
       </c>
-      <c r="H53" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "53", ( Character: "S", Windows1252UrlEncoding: "%53", Utf8Encoding: "%53", HtmlEntityName: "", XmlEntityNumber: "&amp;#83;" ) },</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="54" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A54" s="4">
         <v>54</v>
       </c>
@@ -4489,12 +4273,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#84;</v>
       </c>
-      <c r="H54" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "54", ( Character: "T", Windows1252UrlEncoding: "%54", Utf8Encoding: "%54", HtmlEntityName: "", XmlEntityNumber: "&amp;#84;" ) },</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="55" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A55" s="5">
         <v>55</v>
       </c>
@@ -4515,12 +4295,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#85;</v>
       </c>
-      <c r="H55" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "55", ( Character: "U", Windows1252UrlEncoding: "%55", Utf8Encoding: "%55", HtmlEntityName: "", XmlEntityNumber: "&amp;#85;" ) },</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="56" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A56" s="4">
         <v>56</v>
       </c>
@@ -4541,12 +4317,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#86;</v>
       </c>
-      <c r="H56" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "56", ( Character: "V", Windows1252UrlEncoding: "%56", Utf8Encoding: "%56", HtmlEntityName: "", XmlEntityNumber: "&amp;#86;" ) },</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="57" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A57" s="5">
         <v>57</v>
       </c>
@@ -4567,12 +4339,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#87;</v>
       </c>
-      <c r="H57" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "57", ( Character: "W", Windows1252UrlEncoding: "%57", Utf8Encoding: "%57", HtmlEntityName: "", XmlEntityNumber: "&amp;#87;" ) },</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="58" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A58" s="4">
         <v>58</v>
       </c>
@@ -4593,12 +4361,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#88;</v>
       </c>
-      <c r="H58" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "58", ( Character: "X", Windows1252UrlEncoding: "%58", Utf8Encoding: "%58", HtmlEntityName: "", XmlEntityNumber: "&amp;#88;" ) },</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="59" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A59" s="5">
         <v>59</v>
       </c>
@@ -4619,12 +4383,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#89;</v>
       </c>
-      <c r="H59" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "59", ( Character: "Y", Windows1252UrlEncoding: "%59", Utf8Encoding: "%59", HtmlEntityName: "", XmlEntityNumber: "&amp;#89;" ) },</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="60" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A60" s="4" t="s">
         <v>502</v>
       </c>
@@ -4645,12 +4405,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#90;</v>
       </c>
-      <c r="H60" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "5a", ( Character: "Z", Windows1252UrlEncoding: "%5A", Utf8Encoding: "%5A", HtmlEntityName: "", XmlEntityNumber: "&amp;#90;" ) },</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="61" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A61" s="5" t="s">
         <v>503</v>
       </c>
@@ -4671,12 +4427,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#91;</v>
       </c>
-      <c r="H61" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "5b", ( Character: "[", Windows1252UrlEncoding: "%5B", Utf8Encoding: "%5B", HtmlEntityName: "", XmlEntityNumber: "&amp;#91;" ) },</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="62" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A62" s="4" t="s">
         <v>504</v>
       </c>
@@ -4697,12 +4449,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#92;</v>
       </c>
-      <c r="H62" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "5c", ( Character: "\\", Windows1252UrlEncoding: "%5C", Utf8Encoding: "%5C", HtmlEntityName: "", XmlEntityNumber: "&amp;#92;" ) },</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="63" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A63" s="5" t="s">
         <v>505</v>
       </c>
@@ -4723,12 +4471,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#93;</v>
       </c>
-      <c r="H63" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "5d", ( Character: "]", Windows1252UrlEncoding: "%5D", Utf8Encoding: "%5D", HtmlEntityName: "", XmlEntityNumber: "&amp;#93;" ) },</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="64" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A64" s="4" t="s">
         <v>506</v>
       </c>
@@ -4749,12 +4493,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#94;</v>
       </c>
-      <c r="H64" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "5e", ( Character: "^", Windows1252UrlEncoding: "%5E", Utf8Encoding: "%5E", HtmlEntityName: "", XmlEntityNumber: "&amp;#94;" ) },</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="65" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A65" s="5" t="s">
         <v>507</v>
       </c>
@@ -4775,12 +4515,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#95;</v>
       </c>
-      <c r="H65" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "5f", ( Character: "_", Windows1252UrlEncoding: "%5F", Utf8Encoding: "%5F", HtmlEntityName: "", XmlEntityNumber: "&amp;#95;" ) },</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="66" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A66" s="4">
         <v>60</v>
       </c>
@@ -4801,12 +4537,8 @@
         <f t="shared" si="0"/>
         <v>&amp;#96;</v>
       </c>
-      <c r="H66" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ "60", ( Character: "`", Windows1252UrlEncoding: "%60", Utf8Encoding: "%60", HtmlEntityName: "", XmlEntityNumber: "&amp;#96;" ) },</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="67" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A67" s="5">
         <v>61</v>
       </c>
@@ -4824,15 +4556,11 @@
       </c>
       <c r="F67" s="5"/>
       <c r="G67" s="8" t="str">
-        <f t="shared" ref="G67:G130" si="2">_xlfn.CONCAT("&amp;#",HEX2DEC(A67),";")</f>
+        <f t="shared" ref="G67:G130" si="1">_xlfn.CONCAT("&amp;#",HEX2DEC(A67),";")</f>
         <v>&amp;#97;</v>
       </c>
-      <c r="H67" s="8" t="str">
-        <f t="shared" ref="H67:H130" si="3">_xlfn.CONCAT("{ """, A67, """, ( Character: """, _xlfn.SWITCH(A67, "22", "\""", "5c", "\\", C67), """, Windows1252UrlEncoding: """, D67, """, Utf8Encoding: """, E67, """, HtmlEntityName: """, F67, """, XmlEntityNumber: """, G67, """ ) },")</f>
-        <v>{ "61", ( Character: "a", Windows1252UrlEncoding: "%61", Utf8Encoding: "%61", HtmlEntityName: "", XmlEntityNumber: "&amp;#97;" ) },</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="68" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A68" s="4">
         <v>62</v>
       </c>
@@ -4850,15 +4578,11 @@
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#98;</v>
       </c>
-      <c r="H68" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "62", ( Character: "b", Windows1252UrlEncoding: "%62", Utf8Encoding: "%62", HtmlEntityName: "", XmlEntityNumber: "&amp;#98;" ) },</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="69" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A69" s="5">
         <v>63</v>
       </c>
@@ -4876,15 +4600,11 @@
       </c>
       <c r="F69" s="5"/>
       <c r="G69" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#99;</v>
       </c>
-      <c r="H69" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "63", ( Character: "c", Windows1252UrlEncoding: "%63", Utf8Encoding: "%63", HtmlEntityName: "", XmlEntityNumber: "&amp;#99;" ) },</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="70" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A70" s="4">
         <v>64</v>
       </c>
@@ -4902,15 +4622,11 @@
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#100;</v>
       </c>
-      <c r="H70" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "64", ( Character: "d", Windows1252UrlEncoding: "%64", Utf8Encoding: "%64", HtmlEntityName: "", XmlEntityNumber: "&amp;#100;" ) },</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="71" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A71" s="5">
         <v>65</v>
       </c>
@@ -4928,15 +4644,11 @@
       </c>
       <c r="F71" s="5"/>
       <c r="G71" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#101;</v>
       </c>
-      <c r="H71" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "65", ( Character: "e", Windows1252UrlEncoding: "%65", Utf8Encoding: "%65", HtmlEntityName: "", XmlEntityNumber: "&amp;#101;" ) },</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="72" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A72" s="4">
         <v>66</v>
       </c>
@@ -4954,15 +4666,11 @@
       </c>
       <c r="F72" s="4"/>
       <c r="G72" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#102;</v>
       </c>
-      <c r="H72" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "66", ( Character: "f", Windows1252UrlEncoding: "%66", Utf8Encoding: "%66", HtmlEntityName: "", XmlEntityNumber: "&amp;#102;" ) },</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="73" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A73" s="5">
         <v>67</v>
       </c>
@@ -4980,15 +4688,11 @@
       </c>
       <c r="F73" s="5"/>
       <c r="G73" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#103;</v>
       </c>
-      <c r="H73" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "67", ( Character: "g", Windows1252UrlEncoding: "%67", Utf8Encoding: "%67", HtmlEntityName: "", XmlEntityNumber: "&amp;#103;" ) },</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="74" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A74" s="4">
         <v>68</v>
       </c>
@@ -5006,15 +4710,11 @@
       </c>
       <c r="F74" s="4"/>
       <c r="G74" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#104;</v>
       </c>
-      <c r="H74" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "68", ( Character: "h", Windows1252UrlEncoding: "%68", Utf8Encoding: "%68", HtmlEntityName: "", XmlEntityNumber: "&amp;#104;" ) },</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="75" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A75" s="5">
         <v>69</v>
       </c>
@@ -5032,15 +4732,11 @@
       </c>
       <c r="F75" s="5"/>
       <c r="G75" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#105;</v>
       </c>
-      <c r="H75" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "69", ( Character: "i", Windows1252UrlEncoding: "%69", Utf8Encoding: "%69", HtmlEntityName: "", XmlEntityNumber: "&amp;#105;" ) },</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="76" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A76" s="4" t="s">
         <v>508</v>
       </c>
@@ -5058,15 +4754,11 @@
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#106;</v>
       </c>
-      <c r="H76" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "6a", ( Character: "j", Windows1252UrlEncoding: "%6A", Utf8Encoding: "%6A", HtmlEntityName: "", XmlEntityNumber: "&amp;#106;" ) },</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="77" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A77" s="5" t="s">
         <v>509</v>
       </c>
@@ -5084,15 +4776,11 @@
       </c>
       <c r="F77" s="5"/>
       <c r="G77" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#107;</v>
       </c>
-      <c r="H77" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "6b", ( Character: "k", Windows1252UrlEncoding: "%6B", Utf8Encoding: "%6B", HtmlEntityName: "", XmlEntityNumber: "&amp;#107;" ) },</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="78" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A78" s="4" t="s">
         <v>510</v>
       </c>
@@ -5110,15 +4798,11 @@
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#108;</v>
       </c>
-      <c r="H78" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "6c", ( Character: "l", Windows1252UrlEncoding: "%6C", Utf8Encoding: "%6C", HtmlEntityName: "", XmlEntityNumber: "&amp;#108;" ) },</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="79" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A79" s="5" t="s">
         <v>511</v>
       </c>
@@ -5136,15 +4820,11 @@
       </c>
       <c r="F79" s="5"/>
       <c r="G79" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#109;</v>
       </c>
-      <c r="H79" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "6d", ( Character: "m", Windows1252UrlEncoding: "%6D", Utf8Encoding: "%6D", HtmlEntityName: "", XmlEntityNumber: "&amp;#109;" ) },</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="80" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A80" s="4" t="s">
         <v>512</v>
       </c>
@@ -5162,15 +4842,11 @@
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#110;</v>
       </c>
-      <c r="H80" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "6e", ( Character: "n", Windows1252UrlEncoding: "%6E", Utf8Encoding: "%6E", HtmlEntityName: "", XmlEntityNumber: "&amp;#110;" ) },</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="81" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A81" s="5" t="s">
         <v>513</v>
       </c>
@@ -5188,15 +4864,11 @@
       </c>
       <c r="F81" s="5"/>
       <c r="G81" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#111;</v>
       </c>
-      <c r="H81" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "6f", ( Character: "o", Windows1252UrlEncoding: "%6F", Utf8Encoding: "%6F", HtmlEntityName: "", XmlEntityNumber: "&amp;#111;" ) },</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="82" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A82" s="4">
         <v>70</v>
       </c>
@@ -5214,15 +4886,11 @@
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#112;</v>
       </c>
-      <c r="H82" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "70", ( Character: "p", Windows1252UrlEncoding: "%70", Utf8Encoding: "%70", HtmlEntityName: "", XmlEntityNumber: "&amp;#112;" ) },</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="83" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A83" s="5">
         <v>71</v>
       </c>
@@ -5240,15 +4908,11 @@
       </c>
       <c r="F83" s="5"/>
       <c r="G83" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#113;</v>
       </c>
-      <c r="H83" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "71", ( Character: "q", Windows1252UrlEncoding: "%71", Utf8Encoding: "%71", HtmlEntityName: "", XmlEntityNumber: "&amp;#113;" ) },</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="84" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A84" s="4">
         <v>72</v>
       </c>
@@ -5266,15 +4930,11 @@
       </c>
       <c r="F84" s="4"/>
       <c r="G84" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#114;</v>
       </c>
-      <c r="H84" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "72", ( Character: "r", Windows1252UrlEncoding: "%72", Utf8Encoding: "%72", HtmlEntityName: "", XmlEntityNumber: "&amp;#114;" ) },</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="85" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A85" s="5">
         <v>73</v>
       </c>
@@ -5292,15 +4952,11 @@
       </c>
       <c r="F85" s="5"/>
       <c r="G85" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#115;</v>
       </c>
-      <c r="H85" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "73", ( Character: "s", Windows1252UrlEncoding: "%73", Utf8Encoding: "%73", HtmlEntityName: "", XmlEntityNumber: "&amp;#115;" ) },</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="86" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A86" s="4">
         <v>74</v>
       </c>
@@ -5318,15 +4974,11 @@
       </c>
       <c r="F86" s="4"/>
       <c r="G86" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#116;</v>
       </c>
-      <c r="H86" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "74", ( Character: "t", Windows1252UrlEncoding: "%74", Utf8Encoding: "%74", HtmlEntityName: "", XmlEntityNumber: "&amp;#116;" ) },</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="87" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A87" s="5">
         <v>75</v>
       </c>
@@ -5344,15 +4996,11 @@
       </c>
       <c r="F87" s="5"/>
       <c r="G87" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#117;</v>
       </c>
-      <c r="H87" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "75", ( Character: "u", Windows1252UrlEncoding: "%75", Utf8Encoding: "%75", HtmlEntityName: "", XmlEntityNumber: "&amp;#117;" ) },</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="88" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A88" s="4">
         <v>76</v>
       </c>
@@ -5370,15 +5018,11 @@
       </c>
       <c r="F88" s="4"/>
       <c r="G88" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#118;</v>
       </c>
-      <c r="H88" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "76", ( Character: "v", Windows1252UrlEncoding: "%76", Utf8Encoding: "%76", HtmlEntityName: "", XmlEntityNumber: "&amp;#118;" ) },</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="89" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A89" s="5">
         <v>77</v>
       </c>
@@ -5396,15 +5040,11 @@
       </c>
       <c r="F89" s="5"/>
       <c r="G89" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#119;</v>
       </c>
-      <c r="H89" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "77", ( Character: "w", Windows1252UrlEncoding: "%77", Utf8Encoding: "%77", HtmlEntityName: "", XmlEntityNumber: "&amp;#119;" ) },</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="90" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A90" s="4">
         <v>78</v>
       </c>
@@ -5422,15 +5062,11 @@
       </c>
       <c r="F90" s="4"/>
       <c r="G90" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#120;</v>
       </c>
-      <c r="H90" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "78", ( Character: "x", Windows1252UrlEncoding: "%78", Utf8Encoding: "%78", HtmlEntityName: "", XmlEntityNumber: "&amp;#120;" ) },</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="91" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A91" s="5">
         <v>79</v>
       </c>
@@ -5448,15 +5084,11 @@
       </c>
       <c r="F91" s="5"/>
       <c r="G91" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#121;</v>
       </c>
-      <c r="H91" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "79", ( Character: "y", Windows1252UrlEncoding: "%79", Utf8Encoding: "%79", HtmlEntityName: "", XmlEntityNumber: "&amp;#121;" ) },</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="92" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A92" s="4" t="s">
         <v>514</v>
       </c>
@@ -5474,15 +5106,11 @@
       </c>
       <c r="F92" s="4"/>
       <c r="G92" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#122;</v>
       </c>
-      <c r="H92" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "7a", ( Character: "z", Windows1252UrlEncoding: "%7A", Utf8Encoding: "%7A", HtmlEntityName: "", XmlEntityNumber: "&amp;#122;" ) },</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="93" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A93" s="5" t="s">
         <v>515</v>
       </c>
@@ -5500,15 +5128,11 @@
       </c>
       <c r="F93" s="5"/>
       <c r="G93" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#123;</v>
       </c>
-      <c r="H93" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "7b", ( Character: "{", Windows1252UrlEncoding: "%7B", Utf8Encoding: "%7B", HtmlEntityName: "", XmlEntityNumber: "&amp;#123;" ) },</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="94" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A94" s="4" t="s">
         <v>516</v>
       </c>
@@ -5526,15 +5150,11 @@
       </c>
       <c r="F94" s="4"/>
       <c r="G94" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#124;</v>
       </c>
-      <c r="H94" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "7c", ( Character: "|", Windows1252UrlEncoding: "%7C", Utf8Encoding: "%7C", HtmlEntityName: "", XmlEntityNumber: "&amp;#124;" ) },</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="95" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A95" s="5" t="s">
         <v>517</v>
       </c>
@@ -5552,15 +5172,11 @@
       </c>
       <c r="F95" s="5"/>
       <c r="G95" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#125;</v>
       </c>
-      <c r="H95" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "7d", ( Character: "}", Windows1252UrlEncoding: "%7D", Utf8Encoding: "%7D", HtmlEntityName: "", XmlEntityNumber: "&amp;#125;" ) },</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="96" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A96" s="4" t="s">
         <v>518</v>
       </c>
@@ -5578,15 +5194,11 @@
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#126;</v>
       </c>
-      <c r="H96" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "7e", ( Character: "~", Windows1252UrlEncoding: "%7E", Utf8Encoding: "%7E", HtmlEntityName: "", XmlEntityNumber: "&amp;#126;" ) },</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="97" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A97" s="5" t="s">
         <v>721</v>
       </c>
@@ -5602,15 +5214,11 @@
       </c>
       <c r="F97" s="5"/>
       <c r="G97" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#127;</v>
       </c>
-      <c r="H97" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "7f", ( Character: "", Windows1252UrlEncoding: "%7F", Utf8Encoding: "%7F", HtmlEntityName: "", XmlEntityNumber: "&amp;#127;" ) },</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="98" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A98" s="4" t="s">
         <v>722</v>
       </c>
@@ -5628,15 +5236,11 @@
       </c>
       <c r="F98" s="4"/>
       <c r="G98" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#128;</v>
       </c>
-      <c r="H98" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "80", ( Character: "`", Windows1252UrlEncoding: "%80", Utf8Encoding: "%E2%82%AC", HtmlEntityName: "", XmlEntityNumber: "&amp;#128;" ) },</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="99" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A99" s="5">
         <v>81</v>
       </c>
@@ -5654,15 +5258,11 @@
       </c>
       <c r="F99" s="5"/>
       <c r="G99" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#129;</v>
       </c>
-      <c r="H99" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "81", ( Character: "", Windows1252UrlEncoding: "%81", Utf8Encoding: "%81", HtmlEntityName: "", XmlEntityNumber: "&amp;#129;" ) },</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="100" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A100" s="4" t="s">
         <v>519</v>
       </c>
@@ -5682,15 +5282,11 @@
         <v>836</v>
       </c>
       <c r="G100" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8218;</v>
       </c>
-      <c r="H100" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "201a", ( Character: "‚", Windows1252UrlEncoding: "%82", Utf8Encoding: "%E2%80%9A", HtmlEntityName: "	&amp;sbquo;", XmlEntityNumber: "&amp;#8218;" ) },</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="101" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A101" s="5">
         <v>192</v>
       </c>
@@ -5710,15 +5306,11 @@
         <v>831</v>
       </c>
       <c r="G101" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#402;</v>
       </c>
-      <c r="H101" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "192", ( Character: "ƒ", Windows1252UrlEncoding: "%83", Utf8Encoding: "%C6%92", HtmlEntityName: "	&amp;fnof;", XmlEntityNumber: "&amp;#402;" ) },</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="102" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A102" s="4" t="s">
         <v>520</v>
       </c>
@@ -5738,15 +5330,11 @@
         <v>832</v>
       </c>
       <c r="G102" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8222;</v>
       </c>
-      <c r="H102" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "201e", ( Character: "„", Windows1252UrlEncoding: "%84", Utf8Encoding: "%E2%80%9E", HtmlEntityName: "	&amp;bdquo;", XmlEntityNumber: "&amp;#8222;" ) },</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="103" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A103" s="5">
         <v>2026</v>
       </c>
@@ -5766,15 +5354,11 @@
         <v>835</v>
       </c>
       <c r="G103" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8230;</v>
       </c>
-      <c r="H103" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2026", ( Character: "…", Windows1252UrlEncoding: "%85", Utf8Encoding: "%E2%80%A6", HtmlEntityName: "	&amp;hellip;", XmlEntityNumber: "&amp;#8230;" ) },</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="104" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A104" s="4">
         <v>2020</v>
       </c>
@@ -5794,15 +5378,11 @@
         <v>833</v>
       </c>
       <c r="G104" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8224;</v>
       </c>
-      <c r="H104" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2020", ( Character: "†", Windows1252UrlEncoding: "%86", Utf8Encoding: "%E2%80%A0", HtmlEntityName: "	&amp;dagger;", XmlEntityNumber: "&amp;#8224;" ) },</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="105" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A105" s="5">
         <v>2021</v>
       </c>
@@ -5822,15 +5402,11 @@
         <v>834</v>
       </c>
       <c r="G105" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8225;</v>
       </c>
-      <c r="H105" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2021", ( Character: "‡", Windows1252UrlEncoding: "%87", Utf8Encoding: "%E2%80%A1", HtmlEntityName: "	&amp;Dagger;", XmlEntityNumber: "&amp;#8225;" ) },</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="106" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A106" s="4" t="s">
         <v>521</v>
       </c>
@@ -5850,15 +5426,11 @@
         <v>829</v>
       </c>
       <c r="G106" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#710;</v>
       </c>
-      <c r="H106" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2c6", ( Character: "ˆ", Windows1252UrlEncoding: "%88", Utf8Encoding: "%CB%86", HtmlEntityName: "	&amp;circ;", XmlEntityNumber: "&amp;#710;" ) },</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="107" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A107" s="5">
         <v>2030</v>
       </c>
@@ -5878,15 +5450,11 @@
         <v>827</v>
       </c>
       <c r="G107" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8240;</v>
       </c>
-      <c r="H107" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2030", ( Character: "‰", Windows1252UrlEncoding: "%89", Utf8Encoding: "%E2%80%B0", HtmlEntityName: "	&amp;permil;", XmlEntityNumber: "&amp;#8240;" ) },</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="108" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A108" s="4">
         <v>160</v>
       </c>
@@ -5906,15 +5474,11 @@
         <v>828</v>
       </c>
       <c r="G108" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#352;</v>
       </c>
-      <c r="H108" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "160", ( Character: "Š", Windows1252UrlEncoding: "%8A", Utf8Encoding: "%C5%A0", HtmlEntityName: "	&amp;Scaron;", XmlEntityNumber: "&amp;#352;" ) },</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="109" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A109" s="5">
         <v>2039</v>
       </c>
@@ -5934,15 +5498,11 @@
         <v>762</v>
       </c>
       <c r="G109" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8249;</v>
       </c>
-      <c r="H109" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2039", ( Character: "‹", Windows1252UrlEncoding: "%8B", Utf8Encoding: "%E2%80%B9", HtmlEntityName: "	&amp;lsaquo;", XmlEntityNumber: "&amp;#8249;" ) },</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="110" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A110" s="4">
         <v>152</v>
       </c>
@@ -5962,15 +5522,11 @@
         <v>825</v>
       </c>
       <c r="G110" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#338;</v>
       </c>
-      <c r="H110" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "152", ( Character: "Œ", Windows1252UrlEncoding: "%8C", Utf8Encoding: "%C5%92", HtmlEntityName: "	&amp;OElig;", XmlEntityNumber: "&amp;#338;" ) },</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="111" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A111" s="5" t="s">
         <v>522</v>
       </c>
@@ -5988,15 +5544,11 @@
       </c>
       <c r="F111" s="5"/>
       <c r="G111" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#141;</v>
       </c>
-      <c r="H111" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "8d", ( Character: "", Windows1252UrlEncoding: "%8D", Utf8Encoding: "%C5%8D", HtmlEntityName: "", XmlEntityNumber: "&amp;#141;" ) },</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="112" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A112" s="4" t="s">
         <v>523</v>
       </c>
@@ -6014,15 +5566,11 @@
       </c>
       <c r="F112" s="4"/>
       <c r="G112" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#381;</v>
       </c>
-      <c r="H112" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "17d", ( Character: "Ž", Windows1252UrlEncoding: "%8E", Utf8Encoding: "%C5%BD", HtmlEntityName: "", XmlEntityNumber: "&amp;#381;" ) },</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="113" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A113" s="5" t="s">
         <v>524</v>
       </c>
@@ -6040,15 +5588,11 @@
       </c>
       <c r="F113" s="5"/>
       <c r="G113" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#143;</v>
       </c>
-      <c r="H113" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "8f", ( Character: "", Windows1252UrlEncoding: "%8F", Utf8Encoding: "%8F", HtmlEntityName: "", XmlEntityNumber: "&amp;#143;" ) },</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="114" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A114" s="4">
         <v>90</v>
       </c>
@@ -6066,15 +5610,11 @@
       </c>
       <c r="F114" s="4"/>
       <c r="G114" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#144;</v>
       </c>
-      <c r="H114" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "90", ( Character: "", Windows1252UrlEncoding: "%90", Utf8Encoding: "%C2%90", HtmlEntityName: "", XmlEntityNumber: "&amp;#144;" ) },</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="115" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A115" s="5">
         <v>2018</v>
       </c>
@@ -6094,15 +5634,11 @@
         <v>758</v>
       </c>
       <c r="G115" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8216;</v>
       </c>
-      <c r="H115" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2018", ( Character: "‘", Windows1252UrlEncoding: "%91", Utf8Encoding: "%E2%80%98", HtmlEntityName: "&amp;lsquo;", XmlEntityNumber: "&amp;#8216;" ) },</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="116" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A116" s="4">
         <v>2019</v>
       </c>
@@ -6122,15 +5658,11 @@
         <v>757</v>
       </c>
       <c r="G116" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8217;</v>
       </c>
-      <c r="H116" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2019", ( Character: "’", Windows1252UrlEncoding: "%92", Utf8Encoding: "%E2%80%99", HtmlEntityName: "&amp;rsquo;", XmlEntityNumber: "&amp;#8217;" ) },</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="117" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A117" s="5" t="s">
         <v>525</v>
       </c>
@@ -6150,15 +5682,11 @@
         <v>756</v>
       </c>
       <c r="G117" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8220;</v>
       </c>
-      <c r="H117" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "201c", ( Character: "“", Windows1252UrlEncoding: "%93", Utf8Encoding: "%E2%80%9C", HtmlEntityName: "	&amp;ldquo;", XmlEntityNumber: "&amp;#8220;" ) },</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="118" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A118" s="4" t="s">
         <v>526</v>
       </c>
@@ -6178,15 +5706,11 @@
         <v>755</v>
       </c>
       <c r="G118" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8221;</v>
       </c>
-      <c r="H118" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "201d", ( Character: "”", Windows1252UrlEncoding: "%94", Utf8Encoding: "%E2%80%9D", HtmlEntityName: "	&amp;rdquo;", XmlEntityNumber: "&amp;#8221;" ) },</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="119" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A119" s="5">
         <v>2022</v>
       </c>
@@ -6206,15 +5730,11 @@
         <v>754</v>
       </c>
       <c r="G119" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8226;</v>
       </c>
-      <c r="H119" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2022", ( Character: "•", Windows1252UrlEncoding: "%95", Utf8Encoding: "%E2%80%A2", HtmlEntityName: "	&amp;bull;", XmlEntityNumber: "&amp;#8226;" ) },</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="120" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A120" s="4">
         <v>2013</v>
       </c>
@@ -6234,15 +5754,11 @@
         <v>759</v>
       </c>
       <c r="G120" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8211;</v>
       </c>
-      <c r="H120" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2013", ( Character: "–", Windows1252UrlEncoding: "%96", Utf8Encoding: "%E2%80%93", HtmlEntityName: "	&amp;ndash;", XmlEntityNumber: "&amp;#8211;" ) },</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="121" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A121" s="5">
         <v>2014</v>
       </c>
@@ -6262,15 +5778,11 @@
         <v>760</v>
       </c>
       <c r="G121" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8212;</v>
       </c>
-      <c r="H121" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2014", ( Character: "—", Windows1252UrlEncoding: "%97", Utf8Encoding: "%E2%80%94", HtmlEntityName: "	&amp;mdash;", XmlEntityNumber: "&amp;#8212;" ) },</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="122" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A122" s="4" t="s">
         <v>527</v>
       </c>
@@ -6290,15 +5802,11 @@
         <v>761</v>
       </c>
       <c r="G122" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#732;</v>
       </c>
-      <c r="H122" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2dc", ( Character: "˜", Windows1252UrlEncoding: "%98", Utf8Encoding: "%CB%9C", HtmlEntityName: "&amp;tilde;", XmlEntityNumber: "&amp;#732;" ) },</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="123" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A123" s="5">
         <v>2122</v>
       </c>
@@ -6318,15 +5826,11 @@
         <v>763</v>
       </c>
       <c r="G123" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8482;</v>
       </c>
-      <c r="H123" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "2122", ( Character: "™", Windows1252UrlEncoding: "%99", Utf8Encoding: "%E2%84", HtmlEntityName: "	&amp;trade;", XmlEntityNumber: "&amp;#8482;" ) },</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="124" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A124" s="4">
         <v>161</v>
       </c>
@@ -6346,15 +5850,11 @@
         <v>823</v>
       </c>
       <c r="G124" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#353;</v>
       </c>
-      <c r="H124" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "161", ( Character: "š", Windows1252UrlEncoding: "%9A", Utf8Encoding: "%C5%A1", HtmlEntityName: "	&amp;scaron;", XmlEntityNumber: "&amp;#353;" ) },</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" ht="53.25" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="125" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A125" s="5" t="s">
         <v>528</v>
       </c>
@@ -6374,15 +5874,11 @@
         <v>824</v>
       </c>
       <c r="G125" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#8250;</v>
       </c>
-      <c r="H125" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "203a", ( Character: "›", Windows1252UrlEncoding: "%9B", Utf8Encoding: "%E2%80", HtmlEntityName: "&amp;rsaquo;", XmlEntityNumber: "&amp;#8250;" ) },</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="126" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A126" s="4">
         <v>153</v>
       </c>
@@ -6402,15 +5898,11 @@
         <v>826</v>
       </c>
       <c r="G126" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#339;</v>
       </c>
-      <c r="H126" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "153", ( Character: "œ", Windows1252UrlEncoding: "%9C", Utf8Encoding: "%C5%93", HtmlEntityName: "	&amp;oelig;", XmlEntityNumber: "&amp;#339;" ) },</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="127" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A127" s="5" t="s">
         <v>529</v>
       </c>
@@ -6428,15 +5920,11 @@
       </c>
       <c r="F127" s="5"/>
       <c r="G127" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#157;</v>
       </c>
-      <c r="H127" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "9d", ( Character: "", Windows1252UrlEncoding: "%9D", Utf8Encoding: "%9D", HtmlEntityName: "", XmlEntityNumber: "&amp;#157;" ) },</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="128" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A128" s="4" t="s">
         <v>530</v>
       </c>
@@ -6454,15 +5942,11 @@
       </c>
       <c r="F128" s="4"/>
       <c r="G128" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#382;</v>
       </c>
-      <c r="H128" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "17e", ( Character: "ž", Windows1252UrlEncoding: "%9E", Utf8Encoding: "%C5%BE", HtmlEntityName: "", XmlEntityNumber: "&amp;#382;" ) },</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="129" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A129" s="5">
         <v>178</v>
       </c>
@@ -6482,15 +5966,11 @@
         <v>822</v>
       </c>
       <c r="G129" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#376;</v>
       </c>
-      <c r="H129" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "178", ( Character: "Ÿ", Windows1252UrlEncoding: "%9F", Utf8Encoding: "%C5%B8", HtmlEntityName: "	&amp;Yuml;", XmlEntityNumber: "&amp;#376;" ) },</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="130" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A130" s="4" t="s">
         <v>627</v>
       </c>
@@ -6508,15 +5988,11 @@
         <v>630</v>
       </c>
       <c r="G130" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>&amp;#160;</v>
       </c>
-      <c r="H130" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>{ "a0", ( Character: "", Windows1252UrlEncoding: "%A0", Utf8Encoding: "%C2%A0", HtmlEntityName: "&amp;nbsp;", XmlEntityNumber: "&amp;#160;" ) },</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="131" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A131" s="5" t="s">
         <v>626</v>
       </c>
@@ -6536,15 +6012,11 @@
         <v>753</v>
       </c>
       <c r="G131" s="8" t="str">
-        <f t="shared" ref="G131:G194" si="4">_xlfn.CONCAT("&amp;#",HEX2DEC(A131),";")</f>
+        <f t="shared" ref="G131:G194" si="2">_xlfn.CONCAT("&amp;#",HEX2DEC(A131),";")</f>
         <v>&amp;#161;</v>
       </c>
-      <c r="H131" s="8" t="str">
-        <f t="shared" ref="H131:H194" si="5">_xlfn.CONCAT("{ """, A131, """, ( Character: """, _xlfn.SWITCH(A131, "22", "\""", "5c", "\\", C131), """, Windows1252UrlEncoding: """, D131, """, Utf8Encoding: """, E131, """, HtmlEntityName: """, F131, """, XmlEntityNumber: """, G131, """ ) },")</f>
-        <v>{ "a1", ( Character: "¡", Windows1252UrlEncoding: "%A1", Utf8Encoding: "%C2%A1", HtmlEntityName: "	&amp;iexcl;", XmlEntityNumber: "&amp;#161;" ) },</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="132" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A132" s="4" t="s">
         <v>531</v>
       </c>
@@ -6564,15 +6036,11 @@
         <v>636</v>
       </c>
       <c r="G132" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#162;</v>
       </c>
-      <c r="H132" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "a2", ( Character: "¢", Windows1252UrlEncoding: "%A2", Utf8Encoding: "%C2%A2", HtmlEntityName: "	&amp;cent;", XmlEntityNumber: "&amp;#162;" ) },</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="133" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A133" s="5" t="s">
         <v>532</v>
       </c>
@@ -6592,15 +6060,11 @@
         <v>637</v>
       </c>
       <c r="G133" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#163;</v>
       </c>
-      <c r="H133" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "a3", ( Character: "£", Windows1252UrlEncoding: "%A3", Utf8Encoding: "%C2%A3", HtmlEntityName: "	&amp;pound;", XmlEntityNumber: "&amp;#163;" ) },</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="134" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A134" s="4" t="s">
         <v>533</v>
       </c>
@@ -6620,15 +6084,11 @@
         <v>752</v>
       </c>
       <c r="G134" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#164;</v>
       </c>
-      <c r="H134" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "a4", ( Character: "¤", Windows1252UrlEncoding: "%A4", Utf8Encoding: "%C2%A4", HtmlEntityName: "	&amp;curren;", XmlEntityNumber: "&amp;#164;" ) },</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="135" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A135" s="5" t="s">
         <v>534</v>
       </c>
@@ -6648,15 +6108,11 @@
         <v>638</v>
       </c>
       <c r="G135" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#165;</v>
       </c>
-      <c r="H135" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "a5", ( Character: "¥", Windows1252UrlEncoding: "%A5", Utf8Encoding: "%C2%A5", HtmlEntityName: "	&amp;yen;", XmlEntityNumber: "&amp;#165;" ) },</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="136" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A136" s="4" t="s">
         <v>535</v>
       </c>
@@ -6676,15 +6132,11 @@
         <v>751</v>
       </c>
       <c r="G136" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#166;</v>
       </c>
-      <c r="H136" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "a6", ( Character: "¦", Windows1252UrlEncoding: "%A6", Utf8Encoding: "%C2%A6", HtmlEntityName: "	&amp;brvbar;", XmlEntityNumber: "&amp;#166;" ) },</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="137" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A137" s="5" t="s">
         <v>536</v>
       </c>
@@ -6704,15 +6156,11 @@
         <v>750</v>
       </c>
       <c r="G137" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#167;</v>
       </c>
-      <c r="H137" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "a7", ( Character: "§", Windows1252UrlEncoding: "%A7", Utf8Encoding: "%C2%A7", HtmlEntityName: "	&amp;sect;", XmlEntityNumber: "&amp;#167;" ) },</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="138" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A138" s="4" t="s">
         <v>537</v>
       </c>
@@ -6732,15 +6180,11 @@
         <v>749</v>
       </c>
       <c r="G138" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#168;</v>
       </c>
-      <c r="H138" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "a8", ( Character: "¨", Windows1252UrlEncoding: "%A8", Utf8Encoding: "%C2%A8", HtmlEntityName: "	&amp;uml;", XmlEntityNumber: "&amp;#168;" ) },</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="139" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A139" s="5" t="s">
         <v>538</v>
       </c>
@@ -6760,15 +6204,11 @@
         <v>639</v>
       </c>
       <c r="G139" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#169;</v>
       </c>
-      <c r="H139" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "a9", ( Character: "©", Windows1252UrlEncoding: "%A9", Utf8Encoding: "%C2%A9", HtmlEntityName: "	&amp;copy;", XmlEntityNumber: "&amp;#169;" ) },</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="140" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A140" s="4" t="s">
         <v>539</v>
       </c>
@@ -6788,15 +6228,11 @@
         <v>748</v>
       </c>
       <c r="G140" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#170;</v>
       </c>
-      <c r="H140" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "aa", ( Character: "ª", Windows1252UrlEncoding: "%AA", Utf8Encoding: "%C2%AA", HtmlEntityName: "	&amp;ordf;", XmlEntityNumber: "&amp;#170;" ) },</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="141" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A141" s="5" t="s">
         <v>540</v>
       </c>
@@ -6816,15 +6252,11 @@
         <v>747</v>
       </c>
       <c r="G141" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#171;</v>
       </c>
-      <c r="H141" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "ab", ( Character: "«", Windows1252UrlEncoding: "%AB", Utf8Encoding: "%C2%AB", HtmlEntityName: "	&amp;laquo;", XmlEntityNumber: "&amp;#171;" ) },</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="142" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A142" s="4" t="s">
         <v>541</v>
       </c>
@@ -6844,15 +6276,11 @@
         <v>746</v>
       </c>
       <c r="G142" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#172;</v>
       </c>
-      <c r="H142" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "ac", ( Character: "¬", Windows1252UrlEncoding: "%AC", Utf8Encoding: "%C2%AC", HtmlEntityName: "	&amp;not;", XmlEntityNumber: "&amp;#172;" ) },</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="143" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A143" s="5" t="s">
         <v>542</v>
       </c>
@@ -6872,15 +6300,11 @@
         <v>745</v>
       </c>
       <c r="G143" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#173;</v>
       </c>
-      <c r="H143" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "ad", ( Character: "­", Windows1252UrlEncoding: "%AD", Utf8Encoding: "%C2%AD", HtmlEntityName: "	&amp;shy;", XmlEntityNumber: "&amp;#173;" ) },</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="144" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A144" s="4" t="s">
         <v>543</v>
       </c>
@@ -6900,15 +6324,11 @@
         <v>640</v>
       </c>
       <c r="G144" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#174;</v>
       </c>
-      <c r="H144" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "ae", ( Character: "®", Windows1252UrlEncoding: "%AE", Utf8Encoding: "%C2%AE", HtmlEntityName: "	&amp;reg;", XmlEntityNumber: "&amp;#174;" ) },</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="145" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A145" s="5" t="s">
         <v>544</v>
       </c>
@@ -6928,15 +6348,11 @@
         <v>744</v>
       </c>
       <c r="G145" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#175;</v>
       </c>
-      <c r="H145" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "af", ( Character: "¯", Windows1252UrlEncoding: "%AF", Utf8Encoding: "%C2%AF", HtmlEntityName: "	&amp;macr;", XmlEntityNumber: "&amp;#175;" ) },</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="146" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A146" s="4" t="s">
         <v>545</v>
       </c>
@@ -6956,15 +6372,11 @@
         <v>743</v>
       </c>
       <c r="G146" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#176;</v>
       </c>
-      <c r="H146" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "b0", ( Character: "°", Windows1252UrlEncoding: "%B0", Utf8Encoding: "%C2%B0", HtmlEntityName: "	&amp;deg;", XmlEntityNumber: "&amp;#176;" ) },</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="147" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A147" s="5" t="s">
         <v>546</v>
       </c>
@@ -6984,15 +6396,11 @@
         <v>742</v>
       </c>
       <c r="G147" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#177;</v>
       </c>
-      <c r="H147" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "b1", ( Character: "±", Windows1252UrlEncoding: "%B1", Utf8Encoding: "%C2%B1", HtmlEntityName: "&amp;plusmn;", XmlEntityNumber: "&amp;#177;" ) },</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="148" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A148" s="4" t="s">
         <v>547</v>
       </c>
@@ -7012,15 +6420,11 @@
         <v>741</v>
       </c>
       <c r="G148" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#178;</v>
       </c>
-      <c r="H148" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "b2", ( Character: "²", Windows1252UrlEncoding: "%B2", Utf8Encoding: "%C2%B2", HtmlEntityName: "	&amp;sup2;", XmlEntityNumber: "&amp;#178;" ) },</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="149" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A149" s="5" t="s">
         <v>548</v>
       </c>
@@ -7040,15 +6444,11 @@
         <v>740</v>
       </c>
       <c r="G149" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#179;</v>
       </c>
-      <c r="H149" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "b3", ( Character: "³", Windows1252UrlEncoding: "%B3", Utf8Encoding: "%C2%B3", HtmlEntityName: "	&amp;sup3;", XmlEntityNumber: "&amp;#179;" ) },</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="150" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A150" s="4" t="s">
         <v>549</v>
       </c>
@@ -7068,15 +6468,11 @@
         <v>739</v>
       </c>
       <c r="G150" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#180;</v>
       </c>
-      <c r="H150" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "b4", ( Character: "´", Windows1252UrlEncoding: "%B4", Utf8Encoding: "%C2%B4", HtmlEntityName: "	&amp;acute;", XmlEntityNumber: "&amp;#180;" ) },</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="151" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A151" s="5" t="s">
         <v>550</v>
       </c>
@@ -7096,15 +6492,11 @@
         <v>738</v>
       </c>
       <c r="G151" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#181;</v>
       </c>
-      <c r="H151" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "b5", ( Character: "µ", Windows1252UrlEncoding: "%B5", Utf8Encoding: "%C2%B5", HtmlEntityName: "	&amp;micro;", XmlEntityNumber: "&amp;#181;" ) },</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="152" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A152" s="4" t="s">
         <v>551</v>
       </c>
@@ -7124,15 +6516,11 @@
         <v>737</v>
       </c>
       <c r="G152" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#182;</v>
       </c>
-      <c r="H152" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "b6", ( Character: "¶", Windows1252UrlEncoding: "%B6", Utf8Encoding: "%C2%B6", HtmlEntityName: "	&amp;para;", XmlEntityNumber: "&amp;#182;" ) },</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="153" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A153" s="5" t="s">
         <v>552</v>
       </c>
@@ -7152,15 +6540,11 @@
         <v>838</v>
       </c>
       <c r="G153" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#183;</v>
       </c>
-      <c r="H153" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "b7", ( Character: "·", Windows1252UrlEncoding: "%B7", Utf8Encoding: "%C2%B7", HtmlEntityName: "&amp;middot;", XmlEntityNumber: "&amp;#183;" ) },</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="154" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A154" s="4" t="s">
         <v>553</v>
       </c>
@@ -7180,15 +6564,11 @@
         <v>736</v>
       </c>
       <c r="G154" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#184;</v>
       </c>
-      <c r="H154" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "b8", ( Character: "¸", Windows1252UrlEncoding: "%B8", Utf8Encoding: "%C2%B8", HtmlEntityName: "	&amp;cedil;", XmlEntityNumber: "&amp;#184;" ) },</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="155" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A155" s="5" t="s">
         <v>554</v>
       </c>
@@ -7208,15 +6588,11 @@
         <v>735</v>
       </c>
       <c r="G155" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#185;</v>
       </c>
-      <c r="H155" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "b9", ( Character: "¹", Windows1252UrlEncoding: "%B9", Utf8Encoding: "%C2%B9", HtmlEntityName: "	&amp;sup1;", XmlEntityNumber: "&amp;#185;" ) },</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="156" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A156" s="4" t="s">
         <v>555</v>
       </c>
@@ -7236,15 +6612,11 @@
         <v>734</v>
       </c>
       <c r="G156" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#186;</v>
       </c>
-      <c r="H156" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "ba", ( Character: "º", Windows1252UrlEncoding: "%BA", Utf8Encoding: "%C2%BA", HtmlEntityName: "	&amp;ordm;", XmlEntityNumber: "&amp;#186;" ) },</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="157" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A157" s="5" t="s">
         <v>556</v>
       </c>
@@ -7264,15 +6636,11 @@
         <v>733</v>
       </c>
       <c r="G157" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#187;</v>
       </c>
-      <c r="H157" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "bb", ( Character: "»", Windows1252UrlEncoding: "%BB", Utf8Encoding: "%C2%BB", HtmlEntityName: "	&amp;raquo;", XmlEntityNumber: "&amp;#187;" ) },</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="158" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A158" s="4" t="s">
         <v>557</v>
       </c>
@@ -7292,15 +6660,11 @@
         <v>732</v>
       </c>
       <c r="G158" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#188;</v>
       </c>
-      <c r="H158" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "bc", ( Character: "¼", Windows1252UrlEncoding: "%BC", Utf8Encoding: "%C2%BC", HtmlEntityName: "	&amp;frac14;", XmlEntityNumber: "&amp;#188;" ) },</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="159" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A159" s="5" t="s">
         <v>558</v>
       </c>
@@ -7320,15 +6684,11 @@
         <v>729</v>
       </c>
       <c r="G159" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#189;</v>
       </c>
-      <c r="H159" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "bd", ( Character: "½", Windows1252UrlEncoding: "%BD", Utf8Encoding: "%C2%BD", HtmlEntityName: "&amp;frac12;", XmlEntityNumber: "&amp;#189;" ) },</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="160" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A160" s="4" t="s">
         <v>559</v>
       </c>
@@ -7348,15 +6708,11 @@
         <v>730</v>
       </c>
       <c r="G160" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#190;</v>
       </c>
-      <c r="H160" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "be", ( Character: "¾", Windows1252UrlEncoding: "%BE", Utf8Encoding: "%C2%BE", HtmlEntityName: "	&amp;frac34;", XmlEntityNumber: "&amp;#190;" ) },</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="161" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A161" s="5" t="s">
         <v>560</v>
       </c>
@@ -7376,15 +6732,11 @@
         <v>731</v>
       </c>
       <c r="G161" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#191;</v>
       </c>
-      <c r="H161" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "bf", ( Character: "¿", Windows1252UrlEncoding: "%BF", Utf8Encoding: "%C2%BF", HtmlEntityName: "	&amp;iquest;", XmlEntityNumber: "&amp;#191;" ) },</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="162" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A162" s="4" t="s">
         <v>561</v>
       </c>
@@ -7404,15 +6756,11 @@
         <v>764</v>
       </c>
       <c r="G162" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#192;</v>
       </c>
-      <c r="H162" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "c0", ( Character: "À", Windows1252UrlEncoding: "%C0", Utf8Encoding: "%C3%80", HtmlEntityName: "	&amp;Agrave;", XmlEntityNumber: "&amp;#192;" ) },</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="163" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A163" s="5" t="s">
         <v>562</v>
       </c>
@@ -7432,15 +6780,11 @@
         <v>765</v>
       </c>
       <c r="G163" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#193;</v>
       </c>
-      <c r="H163" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "c1", ( Character: "Á", Windows1252UrlEncoding: "%C1", Utf8Encoding: "%C3%81", HtmlEntityName: "	&amp;Aacute;", XmlEntityNumber: "&amp;#193;" ) },</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="164" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A164" s="4" t="s">
         <v>563</v>
       </c>
@@ -7460,15 +6804,11 @@
         <v>766</v>
       </c>
       <c r="G164" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#194;</v>
       </c>
-      <c r="H164" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "c2", ( Character: "Â", Windows1252UrlEncoding: "%C2", Utf8Encoding: "%C3%82", HtmlEntityName: "	&amp;Acirc;", XmlEntityNumber: "&amp;#194;" ) },</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="165" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A165" s="5" t="s">
         <v>564</v>
       </c>
@@ -7488,15 +6828,11 @@
         <v>767</v>
       </c>
       <c r="G165" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#195;</v>
       </c>
-      <c r="H165" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "c3", ( Character: "Ã", Windows1252UrlEncoding: "%C3", Utf8Encoding: "%C3%83", HtmlEntityName: "	&amp;Atilde;", XmlEntityNumber: "&amp;#195;" ) },</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="166" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A166" s="4" t="s">
         <v>565</v>
       </c>
@@ -7516,15 +6852,11 @@
         <v>768</v>
       </c>
       <c r="G166" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#196;</v>
       </c>
-      <c r="H166" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "c4", ( Character: "Ä", Windows1252UrlEncoding: "%C4", Utf8Encoding: "%C3%84", HtmlEntityName: "	&amp;Auml;", XmlEntityNumber: "&amp;#196;" ) },</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="167" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A167" s="5" t="s">
         <v>566</v>
       </c>
@@ -7544,15 +6876,11 @@
         <v>769</v>
       </c>
       <c r="G167" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#197;</v>
       </c>
-      <c r="H167" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "c5", ( Character: "Å", Windows1252UrlEncoding: "%C5", Utf8Encoding: "%C3%85", HtmlEntityName: "	&amp;Aring;", XmlEntityNumber: "&amp;#197;" ) },</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="168" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A168" s="4" t="s">
         <v>567</v>
       </c>
@@ -7572,15 +6900,11 @@
         <v>723</v>
       </c>
       <c r="G168" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#198;</v>
       </c>
-      <c r="H168" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "c6", ( Character: "Æ", Windows1252UrlEncoding: "%C6", Utf8Encoding: "%C3%86", HtmlEntityName: "&amp;AElig;", XmlEntityNumber: "&amp;#198;" ) },</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="169" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A169" s="5" t="s">
         <v>568</v>
       </c>
@@ -7600,15 +6924,11 @@
         <v>770</v>
       </c>
       <c r="G169" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#199;</v>
       </c>
-      <c r="H169" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "c7", ( Character: "Ç", Windows1252UrlEncoding: "%C7", Utf8Encoding: "%C3%87", HtmlEntityName: "	&amp;Ccedil;", XmlEntityNumber: "&amp;#199;" ) },</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="170" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A170" s="4" t="s">
         <v>569</v>
       </c>
@@ -7628,15 +6948,11 @@
         <v>771</v>
       </c>
       <c r="G170" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#200;</v>
       </c>
-      <c r="H170" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "c8", ( Character: "È", Windows1252UrlEncoding: "%C8", Utf8Encoding: "%C3%88", HtmlEntityName: "	&amp;Egrave;", XmlEntityNumber: "&amp;#200;" ) },</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="171" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A171" s="5" t="s">
         <v>570</v>
       </c>
@@ -7656,15 +6972,11 @@
         <v>724</v>
       </c>
       <c r="G171" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#201;</v>
       </c>
-      <c r="H171" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "c9", ( Character: "É", Windows1252UrlEncoding: "%C9", Utf8Encoding: "%C3%89", HtmlEntityName: "&amp;Eacute;", XmlEntityNumber: "&amp;#201;" ) },</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="172" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A172" s="4" t="s">
         <v>571</v>
       </c>
@@ -7684,15 +6996,11 @@
         <v>725</v>
       </c>
       <c r="G172" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#202;</v>
       </c>
-      <c r="H172" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "ca", ( Character: "Ê", Windows1252UrlEncoding: "%CA", Utf8Encoding: "%C3%8A", HtmlEntityName: "&amp;Ecirc;", XmlEntityNumber: "&amp;#202;" ) },</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="173" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A173" s="5" t="s">
         <v>572</v>
       </c>
@@ -7712,15 +7020,11 @@
         <v>772</v>
       </c>
       <c r="G173" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#203;</v>
       </c>
-      <c r="H173" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "cb", ( Character: "Ë", Windows1252UrlEncoding: "%CB", Utf8Encoding: "%C3%8B", HtmlEntityName: "	&amp;Euml;", XmlEntityNumber: "&amp;#203;" ) },</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="174" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A174" s="4" t="s">
         <v>573</v>
       </c>
@@ -7740,15 +7044,11 @@
         <v>773</v>
       </c>
       <c r="G174" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#204;</v>
       </c>
-      <c r="H174" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "cc", ( Character: "Ì", Windows1252UrlEncoding: "%CC", Utf8Encoding: "%C3%8C", HtmlEntityName: "	&amp;Igrave;", XmlEntityNumber: "&amp;#204;" ) },</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="175" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A175" s="5" t="s">
         <v>574</v>
       </c>
@@ -7768,15 +7068,11 @@
         <v>774</v>
       </c>
       <c r="G175" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#205;</v>
       </c>
-      <c r="H175" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "cd", ( Character: "Í", Windows1252UrlEncoding: "%CD", Utf8Encoding: "%C3%8D", HtmlEntityName: "	&amp;Iacute;", XmlEntityNumber: "&amp;#205;" ) },</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="176" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A176" s="4" t="s">
         <v>575</v>
       </c>
@@ -7796,15 +7092,11 @@
         <v>775</v>
       </c>
       <c r="G176" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#206;</v>
       </c>
-      <c r="H176" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "ce", ( Character: "Î", Windows1252UrlEncoding: "%CE", Utf8Encoding: "%C3%8E", HtmlEntityName: "	&amp;Icirc;", XmlEntityNumber: "&amp;#206;" ) },</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="177" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A177" s="5" t="s">
         <v>576</v>
       </c>
@@ -7824,15 +7116,11 @@
         <v>776</v>
       </c>
       <c r="G177" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#207;</v>
       </c>
-      <c r="H177" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "cf", ( Character: "Ï", Windows1252UrlEncoding: "%CF", Utf8Encoding: "%C3%8F", HtmlEntityName: "	&amp;Iuml;", XmlEntityNumber: "&amp;#207;" ) },</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="178" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A178" s="4" t="s">
         <v>577</v>
       </c>
@@ -7852,15 +7140,11 @@
         <v>777</v>
       </c>
       <c r="G178" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#208;</v>
       </c>
-      <c r="H178" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "d0", ( Character: "Ð", Windows1252UrlEncoding: "%D0", Utf8Encoding: "%C3%90", HtmlEntityName: "	&amp;ETH;", XmlEntityNumber: "&amp;#208;" ) },</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="179" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A179" s="5" t="s">
         <v>578</v>
       </c>
@@ -7880,15 +7164,11 @@
         <v>778</v>
       </c>
       <c r="G179" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#209;</v>
       </c>
-      <c r="H179" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "d1", ( Character: "Ñ", Windows1252UrlEncoding: "%D1", Utf8Encoding: "%C3%91", HtmlEntityName: "	&amp;Ntilde;", XmlEntityNumber: "&amp;#209;" ) },</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="180" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A180" s="4" t="s">
         <v>579</v>
       </c>
@@ -7908,15 +7188,11 @@
         <v>726</v>
       </c>
       <c r="G180" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#210;</v>
       </c>
-      <c r="H180" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "d2", ( Character: "Ò", Windows1252UrlEncoding: "%D2", Utf8Encoding: "%C3%92", HtmlEntityName: "&amp;Ograve;", XmlEntityNumber: "&amp;#210;" ) },</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="181" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A181" s="5" t="s">
         <v>580</v>
       </c>
@@ -7936,15 +7212,11 @@
         <v>779</v>
       </c>
       <c r="G181" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#211;</v>
       </c>
-      <c r="H181" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "d3", ( Character: "Ó", Windows1252UrlEncoding: "%D3", Utf8Encoding: "%C3%93", HtmlEntityName: "	&amp;Oacute;", XmlEntityNumber: "&amp;#211;" ) },</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="182" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A182" s="4" t="s">
         <v>581</v>
       </c>
@@ -7964,15 +7236,11 @@
         <v>780</v>
       </c>
       <c r="G182" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#212;</v>
       </c>
-      <c r="H182" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "d4", ( Character: "Ô", Windows1252UrlEncoding: "%D4", Utf8Encoding: "%C3%94", HtmlEntityName: "	&amp;Ocirc;", XmlEntityNumber: "&amp;#212;" ) },</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="183" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A183" s="5" t="s">
         <v>582</v>
       </c>
@@ -7992,15 +7260,11 @@
         <v>781</v>
       </c>
       <c r="G183" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#213;</v>
       </c>
-      <c r="H183" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "d5", ( Character: "Õ", Windows1252UrlEncoding: "%D5", Utf8Encoding: "%C3%95", HtmlEntityName: "	&amp;Otilde;", XmlEntityNumber: "&amp;#213;" ) },</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="184" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A184" s="4" t="s">
         <v>583</v>
       </c>
@@ -8020,15 +7284,11 @@
         <v>727</v>
       </c>
       <c r="G184" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#214;</v>
       </c>
-      <c r="H184" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "d6", ( Character: "Ö", Windows1252UrlEncoding: "%D6", Utf8Encoding: "%C3%96", HtmlEntityName: "&amp;Ouml;", XmlEntityNumber: "&amp;#214;" ) },</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="185" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A185" s="5" t="s">
         <v>584</v>
       </c>
@@ -8048,15 +7308,11 @@
         <v>821</v>
       </c>
       <c r="G185" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#215;</v>
       </c>
-      <c r="H185" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "d7", ( Character: "×", Windows1252UrlEncoding: "%D7", Utf8Encoding: "%C3%97", HtmlEntityName: "	&amp;times;", XmlEntityNumber: "&amp;#215;" ) },</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="186" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A186" s="4" t="s">
         <v>585</v>
       </c>
@@ -8076,15 +7332,11 @@
         <v>782</v>
       </c>
       <c r="G186" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#216;</v>
       </c>
-      <c r="H186" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "d8", ( Character: "Ø", Windows1252UrlEncoding: "%D8", Utf8Encoding: "%C3%98", HtmlEntityName: "	&amp;Oslash;", XmlEntityNumber: "&amp;#216;" ) },</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="187" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A187" s="5" t="s">
         <v>586</v>
       </c>
@@ -8104,15 +7356,11 @@
         <v>783</v>
       </c>
       <c r="G187" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#217;</v>
       </c>
-      <c r="H187" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "d9", ( Character: "Ù", Windows1252UrlEncoding: "%D9", Utf8Encoding: "%C3%99", HtmlEntityName: "	&amp;Ugrave;", XmlEntityNumber: "&amp;#217;" ) },</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="188" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A188" s="4" t="s">
         <v>587</v>
       </c>
@@ -8132,15 +7380,11 @@
         <v>784</v>
       </c>
       <c r="G188" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#218;</v>
       </c>
-      <c r="H188" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "da", ( Character: "Ú", Windows1252UrlEncoding: "%DA", Utf8Encoding: "%C3%9A", HtmlEntityName: "	&amp;Uacute;", XmlEntityNumber: "&amp;#218;" ) },</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="189" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A189" s="5" t="s">
         <v>588</v>
       </c>
@@ -8160,15 +7404,11 @@
         <v>785</v>
       </c>
       <c r="G189" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#219;</v>
       </c>
-      <c r="H189" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "db", ( Character: "Û", Windows1252UrlEncoding: "%DB", Utf8Encoding: "%C3%9B", HtmlEntityName: "	&amp;Ucirc;", XmlEntityNumber: "&amp;#219;" ) },</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="190" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A190" s="4" t="s">
         <v>589</v>
       </c>
@@ -8188,15 +7428,11 @@
         <v>786</v>
       </c>
       <c r="G190" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#220;</v>
       </c>
-      <c r="H190" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "dc", ( Character: "Ü", Windows1252UrlEncoding: "%DC", Utf8Encoding: "%C3%9C", HtmlEntityName: "	&amp;Uuml;", XmlEntityNumber: "&amp;#220;" ) },</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="191" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A191" s="5" t="s">
         <v>590</v>
       </c>
@@ -8216,15 +7452,11 @@
         <v>787</v>
       </c>
       <c r="G191" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#221;</v>
       </c>
-      <c r="H191" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "dd", ( Character: "Ý", Windows1252UrlEncoding: "%DD", Utf8Encoding: "%C3%9D", HtmlEntityName: "	&amp;Yacute;", XmlEntityNumber: "&amp;#221;" ) },</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="192" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A192" s="4" t="s">
         <v>591</v>
       </c>
@@ -8244,15 +7476,11 @@
         <v>788</v>
       </c>
       <c r="G192" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#222;</v>
       </c>
-      <c r="H192" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "de", ( Character: "Þ", Windows1252UrlEncoding: "%DE", Utf8Encoding: "%C3%9E", HtmlEntityName: "	&amp;THORN;", XmlEntityNumber: "&amp;#222;" ) },</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="193" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A193" s="5" t="s">
         <v>592</v>
       </c>
@@ -8272,15 +7500,11 @@
         <v>789</v>
       </c>
       <c r="G193" s="8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#223;</v>
       </c>
-      <c r="H193" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "df", ( Character: "ß", Windows1252UrlEncoding: "%DF", Utf8Encoding: "%C3%9F", HtmlEntityName: "	&amp;szlig;", XmlEntityNumber: "&amp;#223;" ) },</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="194" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A194" s="4" t="s">
         <v>593</v>
       </c>
@@ -8300,15 +7524,11 @@
         <v>790</v>
       </c>
       <c r="G194" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&amp;#224;</v>
       </c>
-      <c r="H194" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>{ "e0", ( Character: "à", Windows1252UrlEncoding: "%E0", Utf8Encoding: "%C3%A0", HtmlEntityName: "	&amp;agrave;", XmlEntityNumber: "&amp;#224;" ) },</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="195" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A195" s="5" t="s">
         <v>594</v>
       </c>
@@ -8328,15 +7548,11 @@
         <v>791</v>
       </c>
       <c r="G195" s="8" t="str">
-        <f t="shared" ref="G195:G225" si="6">_xlfn.CONCAT("&amp;#",HEX2DEC(A195),";")</f>
+        <f t="shared" ref="G195:G225" si="3">_xlfn.CONCAT("&amp;#",HEX2DEC(A195),";")</f>
         <v>&amp;#225;</v>
       </c>
-      <c r="H195" s="8" t="str">
-        <f t="shared" ref="H195:H225" si="7">_xlfn.CONCAT("{ """, A195, """, ( Character: """, _xlfn.SWITCH(A195, "22", "\""", "5c", "\\", C195), """, Windows1252UrlEncoding: """, D195, """, Utf8Encoding: """, E195, """, HtmlEntityName: """, F195, """, XmlEntityNumber: """, G195, """ ) },")</f>
-        <v>{ "e1", ( Character: "á", Windows1252UrlEncoding: "%E1", Utf8Encoding: "%C3%A1", HtmlEntityName: "	&amp;aacute;", XmlEntityNumber: "&amp;#225;" ) },</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="196" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A196" s="4" t="s">
         <v>595</v>
       </c>
@@ -8356,15 +7572,11 @@
         <v>792</v>
       </c>
       <c r="G196" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#226;</v>
       </c>
-      <c r="H196" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "e2", ( Character: "â", Windows1252UrlEncoding: "%E2", Utf8Encoding: "%C3%A2", HtmlEntityName: "	&amp;acirc;", XmlEntityNumber: "&amp;#226;" ) },</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="197" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A197" s="5" t="s">
         <v>596</v>
       </c>
@@ -8384,15 +7596,11 @@
         <v>728</v>
       </c>
       <c r="G197" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#227;</v>
       </c>
-      <c r="H197" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "e3", ( Character: "ã", Windows1252UrlEncoding: "%E3", Utf8Encoding: "%C3%A3", HtmlEntityName: "&amp;atilde;", XmlEntityNumber: "&amp;#227;" ) },</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="198" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A198" s="4" t="s">
         <v>597</v>
       </c>
@@ -8412,15 +7620,11 @@
         <v>793</v>
       </c>
       <c r="G198" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#228;</v>
       </c>
-      <c r="H198" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "e4", ( Character: "ä", Windows1252UrlEncoding: "%E4", Utf8Encoding: "%C3%A4", HtmlEntityName: "	&amp;auml;", XmlEntityNumber: "&amp;#228;" ) },</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="199" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A199" s="5" t="s">
         <v>598</v>
       </c>
@@ -8440,15 +7644,11 @@
         <v>794</v>
       </c>
       <c r="G199" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#229;</v>
       </c>
-      <c r="H199" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "e5", ( Character: "å", Windows1252UrlEncoding: "%E5", Utf8Encoding: "%C3%A5", HtmlEntityName: "	&amp;aring;", XmlEntityNumber: "&amp;#229;" ) },</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="200" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A200" s="4" t="s">
         <v>599</v>
       </c>
@@ -8468,15 +7668,11 @@
         <v>795</v>
       </c>
       <c r="G200" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#230;</v>
       </c>
-      <c r="H200" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "e6", ( Character: "æ", Windows1252UrlEncoding: "%E6", Utf8Encoding: "%C3%A6", HtmlEntityName: "	&amp;aelig;", XmlEntityNumber: "&amp;#230;" ) },</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="201" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A201" s="5" t="s">
         <v>600</v>
       </c>
@@ -8496,15 +7692,11 @@
         <v>796</v>
       </c>
       <c r="G201" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#231;</v>
       </c>
-      <c r="H201" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "e7", ( Character: "ç", Windows1252UrlEncoding: "%E7", Utf8Encoding: "%C3%A7", HtmlEntityName: "	&amp;ccedil;", XmlEntityNumber: "&amp;#231;" ) },</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="202" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A202" s="4" t="s">
         <v>601</v>
       </c>
@@ -8524,15 +7716,11 @@
         <v>797</v>
       </c>
       <c r="G202" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#232;</v>
       </c>
-      <c r="H202" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "e8", ( Character: "è", Windows1252UrlEncoding: "%E8", Utf8Encoding: "%C3%A8", HtmlEntityName: "	&amp;egrave;", XmlEntityNumber: "&amp;#232;" ) },</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="203" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A203" s="5" t="s">
         <v>602</v>
       </c>
@@ -8552,15 +7740,11 @@
         <v>798</v>
       </c>
       <c r="G203" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#233;</v>
       </c>
-      <c r="H203" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "e9", ( Character: "é", Windows1252UrlEncoding: "%E9", Utf8Encoding: "%C3%A9", HtmlEntityName: "	&amp;eacute;", XmlEntityNumber: "&amp;#233;" ) },</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="204" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A204" s="4" t="s">
         <v>603</v>
       </c>
@@ -8580,15 +7764,11 @@
         <v>799</v>
       </c>
       <c r="G204" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#234;</v>
       </c>
-      <c r="H204" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "ea", ( Character: "ê", Windows1252UrlEncoding: "%EA", Utf8Encoding: "%C3%AA", HtmlEntityName: "	&amp;ecirc;", XmlEntityNumber: "&amp;#234;" ) },</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="205" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A205" s="5" t="s">
         <v>604</v>
       </c>
@@ -8608,15 +7788,11 @@
         <v>800</v>
       </c>
       <c r="G205" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#235;</v>
       </c>
-      <c r="H205" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "eb", ( Character: "ë", Windows1252UrlEncoding: "%EB", Utf8Encoding: "%C3%AB", HtmlEntityName: "	&amp;euml;", XmlEntityNumber: "&amp;#235;" ) },</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="206" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A206" s="4" t="s">
         <v>605</v>
       </c>
@@ -8636,15 +7812,11 @@
         <v>801</v>
       </c>
       <c r="G206" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#236;</v>
       </c>
-      <c r="H206" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "ec", ( Character: "ì", Windows1252UrlEncoding: "%EC", Utf8Encoding: "%C3%AC", HtmlEntityName: "	&amp;igrave;", XmlEntityNumber: "&amp;#236;" ) },</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="207" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A207" s="5" t="s">
         <v>606</v>
       </c>
@@ -8664,15 +7836,11 @@
         <v>802</v>
       </c>
       <c r="G207" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#237;</v>
       </c>
-      <c r="H207" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "ed", ( Character: "í", Windows1252UrlEncoding: "%ED", Utf8Encoding: "%C3%AD", HtmlEntityName: "	&amp;iacute;", XmlEntityNumber: "&amp;#237;" ) },</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="208" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A208" s="4" t="s">
         <v>607</v>
       </c>
@@ -8692,15 +7860,11 @@
         <v>803</v>
       </c>
       <c r="G208" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#238;</v>
       </c>
-      <c r="H208" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "ee", ( Character: "î", Windows1252UrlEncoding: "%EE", Utf8Encoding: "%C3%AE", HtmlEntityName: "	&amp;icirc;", XmlEntityNumber: "&amp;#238;" ) },</v>
-      </c>
-    </row>
-    <row r="209" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="209" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A209" s="5" t="s">
         <v>608</v>
       </c>
@@ -8720,15 +7884,11 @@
         <v>804</v>
       </c>
       <c r="G209" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#239;</v>
       </c>
-      <c r="H209" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "ef", ( Character: "ï", Windows1252UrlEncoding: "%EF", Utf8Encoding: "%C3%AF", HtmlEntityName: "	&amp;iuml;", XmlEntityNumber: "&amp;#239;" ) },</v>
-      </c>
-    </row>
-    <row r="210" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="210" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A210" s="4" t="s">
         <v>609</v>
       </c>
@@ -8748,15 +7908,11 @@
         <v>805</v>
       </c>
       <c r="G210" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#240;</v>
       </c>
-      <c r="H210" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "f0", ( Character: "ð", Windows1252UrlEncoding: "%F0", Utf8Encoding: "%C3%B0", HtmlEntityName: "	&amp;eth;", XmlEntityNumber: "&amp;#240;" ) },</v>
-      </c>
-    </row>
-    <row r="211" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="211" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A211" s="5" t="s">
         <v>610</v>
       </c>
@@ -8776,15 +7932,11 @@
         <v>806</v>
       </c>
       <c r="G211" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#241;</v>
       </c>
-      <c r="H211" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "f1", ( Character: "ñ", Windows1252UrlEncoding: "%F1", Utf8Encoding: "%C3%B1", HtmlEntityName: "	&amp;ntilde;", XmlEntityNumber: "&amp;#241;" ) },</v>
-      </c>
-    </row>
-    <row r="212" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="212" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A212" s="4" t="s">
         <v>611</v>
       </c>
@@ -8804,15 +7956,11 @@
         <v>807</v>
       </c>
       <c r="G212" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#242;</v>
       </c>
-      <c r="H212" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "f2", ( Character: "ò", Windows1252UrlEncoding: "%F2", Utf8Encoding: "%C3%B2", HtmlEntityName: "	&amp;ograve;", XmlEntityNumber: "&amp;#242;" ) },</v>
-      </c>
-    </row>
-    <row r="213" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="213" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A213" s="5" t="s">
         <v>612</v>
       </c>
@@ -8832,15 +7980,11 @@
         <v>808</v>
       </c>
       <c r="G213" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#243;</v>
       </c>
-      <c r="H213" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "f3", ( Character: "ó", Windows1252UrlEncoding: "%F3", Utf8Encoding: "%C3%B3", HtmlEntityName: "	&amp;oacute;", XmlEntityNumber: "&amp;#243;" ) },</v>
-      </c>
-    </row>
-    <row r="214" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="214" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A214" s="4" t="s">
         <v>613</v>
       </c>
@@ -8860,15 +8004,11 @@
         <v>809</v>
       </c>
       <c r="G214" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#244;</v>
       </c>
-      <c r="H214" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "f4", ( Character: "ô", Windows1252UrlEncoding: "%F4", Utf8Encoding: "%C3%B4", HtmlEntityName: "	&amp;ocirc;", XmlEntityNumber: "&amp;#244;" ) },</v>
-      </c>
-    </row>
-    <row r="215" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="215" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A215" s="5" t="s">
         <v>614</v>
       </c>
@@ -8888,15 +8028,11 @@
         <v>810</v>
       </c>
       <c r="G215" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#245;</v>
       </c>
-      <c r="H215" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "f5", ( Character: "õ", Windows1252UrlEncoding: "%F5", Utf8Encoding: "%C3%B5", HtmlEntityName: "	&amp;otilde;", XmlEntityNumber: "&amp;#245;" ) },</v>
-      </c>
-    </row>
-    <row r="216" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="216" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A216" s="4" t="s">
         <v>615</v>
       </c>
@@ -8916,15 +8052,11 @@
         <v>811</v>
       </c>
       <c r="G216" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#246;</v>
       </c>
-      <c r="H216" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "f6", ( Character: "ö", Windows1252UrlEncoding: "%F6", Utf8Encoding: "%C3%B6", HtmlEntityName: "	&amp;ouml;", XmlEntityNumber: "&amp;#246;" ) },</v>
-      </c>
-    </row>
-    <row r="217" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="217" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A217" s="5" t="s">
         <v>616</v>
       </c>
@@ -8944,15 +8076,11 @@
         <v>820</v>
       </c>
       <c r="G217" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#247;</v>
       </c>
-      <c r="H217" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "f7", ( Character: "÷", Windows1252UrlEncoding: "%F7", Utf8Encoding: "%C3%B7", HtmlEntityName: "	&amp;divide;", XmlEntityNumber: "&amp;#247;" ) },</v>
-      </c>
-    </row>
-    <row r="218" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="218" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A218" s="4" t="s">
         <v>617</v>
       </c>
@@ -8972,15 +8100,11 @@
         <v>812</v>
       </c>
       <c r="G218" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#248;</v>
       </c>
-      <c r="H218" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "f8", ( Character: "ø", Windows1252UrlEncoding: "%F8", Utf8Encoding: "%C3%B8", HtmlEntityName: "	&amp;oslash;", XmlEntityNumber: "&amp;#248;" ) },</v>
-      </c>
-    </row>
-    <row r="219" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="219" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A219" s="5" t="s">
         <v>618</v>
       </c>
@@ -9000,15 +8124,11 @@
         <v>813</v>
       </c>
       <c r="G219" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#249;</v>
       </c>
-      <c r="H219" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "f9", ( Character: "ù", Windows1252UrlEncoding: "%F9", Utf8Encoding: "%C3%B9", HtmlEntityName: "	&amp;ugrave;", XmlEntityNumber: "&amp;#249;" ) },</v>
-      </c>
-    </row>
-    <row r="220" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="220" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A220" s="4" t="s">
         <v>619</v>
       </c>
@@ -9028,15 +8148,11 @@
         <v>814</v>
       </c>
       <c r="G220" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#250;</v>
       </c>
-      <c r="H220" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "fa", ( Character: "ú", Windows1252UrlEncoding: "%FA", Utf8Encoding: "%C3%BA", HtmlEntityName: "	&amp;uacute;", XmlEntityNumber: "&amp;#250;" ) },</v>
-      </c>
-    </row>
-    <row r="221" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="221" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A221" s="5" t="s">
         <v>620</v>
       </c>
@@ -9056,15 +8172,11 @@
         <v>815</v>
       </c>
       <c r="G221" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#251;</v>
       </c>
-      <c r="H221" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "fb", ( Character: "û", Windows1252UrlEncoding: "%FB", Utf8Encoding: "%C3%BB", HtmlEntityName: "	&amp;ucirc;", XmlEntityNumber: "&amp;#251;" ) },</v>
-      </c>
-    </row>
-    <row r="222" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="222" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A222" s="4" t="s">
         <v>621</v>
       </c>
@@ -9084,15 +8196,11 @@
         <v>816</v>
       </c>
       <c r="G222" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#252;</v>
       </c>
-      <c r="H222" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "fc", ( Character: "ü", Windows1252UrlEncoding: "%FC", Utf8Encoding: "%C3%BC", HtmlEntityName: "	&amp;uuml;", XmlEntityNumber: "&amp;#252;" ) },</v>
-      </c>
-    </row>
-    <row r="223" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="223" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A223" s="5" t="s">
         <v>622</v>
       </c>
@@ -9112,15 +8220,11 @@
         <v>817</v>
       </c>
       <c r="G223" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#253;</v>
       </c>
-      <c r="H223" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "fd", ( Character: "ý", Windows1252UrlEncoding: "%FD", Utf8Encoding: "%C3%BD", HtmlEntityName: "	&amp;yacute;", XmlEntityNumber: "&amp;#253;" ) },</v>
-      </c>
-    </row>
-    <row r="224" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="224" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A224" s="4" t="s">
         <v>623</v>
       </c>
@@ -9140,15 +8244,11 @@
         <v>818</v>
       </c>
       <c r="G224" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#254;</v>
       </c>
-      <c r="H224" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "fe", ( Character: "þ", Windows1252UrlEncoding: "%FE", Utf8Encoding: "%C3%BE", HtmlEntityName: "	&amp;thorn;", XmlEntityNumber: "&amp;#254;" ) },</v>
-      </c>
-    </row>
-    <row r="225" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="225" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A225" s="6" t="s">
         <v>624</v>
       </c>
@@ -9168,20 +8268,16 @@
         <v>819</v>
       </c>
       <c r="G225" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>&amp;#255;</v>
-      </c>
-      <c r="H225" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v>{ "ff", ( Character: "ÿ", Windows1252UrlEncoding: "%FF", Utf8Encoding: "%C3%BF", HtmlEntityName: "	&amp;yuml;", XmlEntityNumber: "&amp;#255;" ) },</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I1" r:id="rId1" xr:uid="{3A311B9A-34D9-4C4B-A0A1-DBA569BCCD07}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{1F3FFF4B-92A7-41DB-8268-22ECA646EC72}"/>
-    <hyperlink ref="I3" r:id="rId3" xr:uid="{D614B9C3-26CA-4DF1-95C6-F1B7C8567C6E}"/>
-    <hyperlink ref="I4" r:id="rId4" xr:uid="{5A21D1F7-CBC4-481D-B827-44324D5D0866}"/>
+    <hyperlink ref="H1" r:id="rId1" xr:uid="{3A311B9A-34D9-4C4B-A0A1-DBA569BCCD07}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{1F3FFF4B-92A7-41DB-8268-22ECA646EC72}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{D614B9C3-26CA-4DF1-95C6-F1B7C8567C6E}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{5A21D1F7-CBC4-481D-B827-44324D5D0866}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
resolves #96 :pencil2: :gear:
</commit_message>
<xml_diff>
--- a/SonghayCore.Tests/xlsx/latin-glyphs.xlsx
+++ b/SonghayCore.Tests/xlsx/latin-glyphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\~shares\sourceRoot\SonghayCore\SonghayCore.Tests\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1520FA8E-27D7-41FB-B175-885228AA55C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF4F94C-E39D-4778-824D-E7A77985C010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28980" yWindow="465" windowWidth="28530" windowHeight="14910" xr2:uid="{37D4E14C-789D-4D3D-87AC-A7379466EBE7}"/>
+    <workbookView xWindow="29235" yWindow="465" windowWidth="27885" windowHeight="14820" xr2:uid="{37D4E14C-789D-4D3D-87AC-A7379466EBE7}"/>
   </bookViews>
   <sheets>
     <sheet name="latin-glyphs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="867">
   <si>
     <t>Character</t>
   </si>
@@ -2583,6 +2583,57 @@
   </si>
   <si>
     <t>22</t>
+  </si>
+  <si>
+    <t>x20ac</t>
+  </si>
+  <si>
+    <t>Currency Symbols</t>
+  </si>
+  <si>
+    <t>€</t>
+  </si>
+  <si>
+    <t>&amp;euro;</t>
+  </si>
+  <si>
+    <t>&amp;#8364;</t>
+  </si>
+  <si>
+    <t>₣</t>
+  </si>
+  <si>
+    <t>x20a3</t>
+  </si>
+  <si>
+    <t>%E2%82%A3</t>
+  </si>
+  <si>
+    <t>&amp;#8355;</t>
+  </si>
+  <si>
+    <t>₤</t>
+  </si>
+  <si>
+    <t>%E2%82%A4</t>
+  </si>
+  <si>
+    <t>x20a4</t>
+  </si>
+  <si>
+    <t>&amp;#8356;</t>
+  </si>
+  <si>
+    <t>₹</t>
+  </si>
+  <si>
+    <t>%E2%82%B9</t>
+  </si>
+  <si>
+    <t>x20b9</t>
+  </si>
+  <si>
+    <t>&amp;#8377;</t>
   </si>
 </sst>
 </file>
@@ -3044,10 +3095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624E43A4-11C6-4DF9-8BF5-916BD7383648}">
-  <dimension ref="A1:H225"/>
+  <dimension ref="A1:H229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="A230" sqref="A230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -8272,6 +8323,84 @@
         <v>&amp;#255;</v>
       </c>
     </row>
+    <row r="226" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A226" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="D226" s="4"/>
+      <c r="E226" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F226" s="4" t="s">
+        <v>853</v>
+      </c>
+      <c r="G226" s="7" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A227" s="6" t="s">
+        <v>856</v>
+      </c>
+      <c r="B227" s="6" t="s">
+        <v>851</v>
+      </c>
+      <c r="C227" s="6" t="s">
+        <v>855</v>
+      </c>
+      <c r="D227" s="6"/>
+      <c r="E227" s="6" t="s">
+        <v>857</v>
+      </c>
+      <c r="F227" s="6"/>
+      <c r="G227" s="9" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A228" s="4" t="s">
+        <v>861</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="C228" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="D228" s="4"/>
+      <c r="E228" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="F228" s="4"/>
+      <c r="G228" s="7" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A229" s="6" t="s">
+        <v>865</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>851</v>
+      </c>
+      <c r="C229" s="6" t="s">
+        <v>863</v>
+      </c>
+      <c r="D229" s="6"/>
+      <c r="E229" s="6" t="s">
+        <v>864</v>
+      </c>
+      <c r="F229" s="6"/>
+      <c r="G229" s="9" t="s">
+        <v>866</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H1" r:id="rId1" xr:uid="{3A311B9A-34D9-4C4B-A0A1-DBA569BCCD07}"/>

</xml_diff>